<commit_message>
Docs, comments and testing added
</commit_message>
<xml_diff>
--- a/documentos/Planner.xlsx
+++ b/documentos/Planner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cotizadortunalitec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Uni\Uni\Decimo semestre\Proyecto integrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{526068E4-50FF-401E-A5A2-55692806FBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEF2DA3-4618-4FF6-B4F9-55921BC177AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBD1E2C6-BC2C-4C4C-A73D-A878FF44D355}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$F$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>Como un…</t>
   </si>
@@ -139,6 +139,30 @@
   </si>
   <si>
     <t>Tiempo total (hrs)</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Cotizaciones correctas de cortinas</t>
+  </si>
+  <si>
+    <t>Cotizar una palillería</t>
+  </si>
+  <si>
+    <t>Ver productos en una orden</t>
+  </si>
+  <si>
+    <t>Ver detalles de producto al crearlo</t>
+  </si>
+  <si>
+    <t>Registro de usuarios</t>
+  </si>
+  <si>
+    <t>Eliminar productos de una orden</t>
+  </si>
+  <si>
+    <t>Ver el formulario de producto en una sola pagina</t>
   </si>
 </sst>
 </file>
@@ -202,7 +226,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFB173C-E595-47EE-AA08-AEA526F9837F}">
-  <dimension ref="B2:F26"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +639,7 @@
     <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -632,7 +656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -649,7 +673,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -666,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -683,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -700,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
@@ -717,7 +741,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
@@ -734,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
@@ -751,7 +775,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
@@ -768,7 +792,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
@@ -785,7 +809,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
@@ -802,41 +826,47 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7">
-        <v>3</v>
-      </c>
-      <c r="E13" s="7">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="7">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>4</v>
-      </c>
-      <c r="F14" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
@@ -853,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
@@ -870,172 +900,306 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4</v>
+      </c>
+      <c r="F17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4</v>
+      </c>
+      <c r="F19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6">
+        <v>8</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>12</v>
+      </c>
+      <c r="F22" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="7">
+        <v>3</v>
+      </c>
+      <c r="E23" s="7">
+        <v>20</v>
+      </c>
+      <c r="F23" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="1">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="1">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
         <v>5</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F25" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="1">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
         <v>6</v>
       </c>
-      <c r="F19" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="1">
-        <v>2</v>
-      </c>
-      <c r="E23" s="1">
-        <v>4</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="1">
-        <v>4</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E32" s="1">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E26" s="2" t="s">
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="3">
-        <f>SUM(F3:F25)</f>
-        <v>45</v>
+      <c r="F33" s="3">
+        <f>SUM(F3:F32)</f>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F26" xr:uid="{4BCE649D-6229-42BA-B504-D31134B72613}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F26">
-      <sortCondition descending="1" ref="D2:D26"/>
+  <autoFilter ref="B2:F33" xr:uid="{4BCE649D-6229-42BA-B504-D31134B72613}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F33">
+      <sortCondition descending="1" ref="D2:D33"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>